<commit_message>
Add new CSV files for microplastic sinks and update exporter to save results
</commit_message>
<xml_diff>
--- a/finale_results.xlsx
+++ b/finale_results.xlsx
@@ -8,6 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Polymer_Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="PA" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="PET" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="PS" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4068,4 +4071,157 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total Sum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Macro</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.1302159545613743</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Micro</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>86.02591692139549</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total Sum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Macro</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>432.9431841512236</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Micro</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>266.268074969384</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Total Sum</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Macro</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>13.36698075189867</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Micro</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>39.45174307950305</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add emission factor calculations and update Excel export functionality
</commit_message>
<xml_diff>
--- a/finale_results.xlsx
+++ b/finale_results.xlsx
@@ -11,6 +11,7 @@
     <sheet name="PA" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="PET" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="PS" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Emission_Factors" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4224,4 +4225,165 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>District</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Emission Factor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Chemnitz, Stadt</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.00055956</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Erzgebirgskreis</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0.00072968</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Mittelsachsen</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.00067033</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Vogtlandkreis</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.00049543</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Zwickau</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.00069221</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Dresden, Stadt</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.00126389</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Bautzen</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.00066184</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Görlitz</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.00055464</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Meißen</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.0005383</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Sächsische Schweiz-Osterzgebirge</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.00054913</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Leipzig, Stadt</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.00138366</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Leipzig</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.00058387</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Nordsachsen</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.00044573</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>